<commit_message>
fix(script): Prevent duplicate headers on ingredients page
The Python script responsible for generating the ingredients page was incorrectly creating extra, empty table headers.

The root cause was an imprecise check (`if 'Ingrediens' in str(...)`) that would trigger not only on the actual header row but also on any ingredient name or empty separator row in the Excel sheet that contained the substring "Ingrediens".

This has been resolved by changing the condition to a strict equality check (`if str(...).strip() == 'Ingrediens'`). This ensures that only the exact header row will now generate a table header, making the parsing logic more robust and preventing future edge-case errors.
</commit_message>
<xml_diff>
--- a/data/laboratorie_data.xlsx
+++ b/data/laboratorie_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvmad\Desktop\Ditz3ns-Ice-Cream-Lab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E04B66-6E81-4F05-9F4F-C168780C070D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF753627-54BD-4A63-9A96-C7179AC4D1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,10 +27,10 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Proteinpulvere" guid="{2D050267-7263-4CD4-97DE-20ADEF3AA056}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Kopi af Proteinpulvere" guid="{BFC8CB06-61D4-4AB5-8D7C-32259655DEAE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Sødemidler &amp; Stabilisatorer" guid="{DDEA0034-8075-451D-A031-0121E8381F0F}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Pulver-baserede Smagsgivere" guid="{78FFC831-1D0F-4AD8-8D5F-BA4B980A515D}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Sødemidler &amp; Stabilisatorer" guid="{DDEA0034-8075-451D-A031-0121E8381F0F}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Kopi af Proteinpulvere" guid="{BFC8CB06-61D4-4AB5-8D7C-32259655DEAE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Proteinpulvere" guid="{2D050267-7263-4CD4-97DE-20ADEF3AA056}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="660">
   <si>
     <t>Velkommen til Ditz3n's Ninja CREAMi Laboratorium! 🍦</t>
   </si>
@@ -2157,12 +2157,6 @@
     <t>Total:</t>
   </si>
   <si>
-    <t>Test Ingrediens</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>Milbona High Protein Vanilla Cottage Cheese</t>
   </si>
 </sst>
@@ -2172,7 +2166,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -2727,30 +2721,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2768,17 +2746,33 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="18" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3046,27 +3040,27 @@
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:8" ht="50.25" customHeight="1">
-      <c r="A1" s="114" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
+      <c r="A1" s="130" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="30.75" customHeight="1">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" ht="12.75">
@@ -3080,10 +3074,10 @@
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A4" s="113" t="s">
+      <c r="A4" s="129" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="112"/>
+      <c r="B4" s="128"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -3092,15 +3086,15 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" ht="12.75">
-      <c r="A5" s="111" t="s">
+      <c r="A5" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="112"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
+      <c r="B5" s="128"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="12.75">
@@ -3114,11 +3108,11 @@
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A7" s="113" t="s">
+      <c r="A7" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="128"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -3126,15 +3120,15 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="12.75">
-      <c r="A8" s="111" t="s">
+      <c r="A8" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="112"/>
-      <c r="C8" s="112"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
-      <c r="G8" s="112"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="128"/>
+      <c r="D8" s="128"/>
+      <c r="E8" s="128"/>
+      <c r="F8" s="128"/>
+      <c r="G8" s="128"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="12.75">
@@ -3148,10 +3142,10 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A10" s="113" t="s">
+      <c r="A10" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="112"/>
+      <c r="B10" s="128"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -3160,15 +3154,15 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="12.75">
-      <c r="A11" s="111" t="s">
+      <c r="A11" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="112"/>
-      <c r="C11" s="112"/>
-      <c r="D11" s="112"/>
-      <c r="E11" s="112"/>
-      <c r="F11" s="112"/>
-      <c r="G11" s="112"/>
+      <c r="B11" s="128"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="128"/>
+      <c r="F11" s="128"/>
+      <c r="G11" s="128"/>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="12.75">
@@ -3182,11 +3176,11 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A13" s="113" t="s">
+      <c r="A13" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="112"/>
-      <c r="C13" s="112"/>
+      <c r="B13" s="128"/>
+      <c r="C13" s="128"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -3194,15 +3188,15 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" ht="12.75">
-      <c r="A14" s="111" t="s">
+      <c r="A14" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="112"/>
-      <c r="C14" s="112"/>
-      <c r="D14" s="112"/>
-      <c r="E14" s="112"/>
-      <c r="F14" s="112"/>
-      <c r="G14" s="112"/>
+      <c r="B14" s="128"/>
+      <c r="C14" s="128"/>
+      <c r="D14" s="128"/>
+      <c r="E14" s="128"/>
+      <c r="F14" s="128"/>
+      <c r="G14" s="128"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="12.75">
@@ -3265,11 +3259,11 @@
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="12.75">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -3455,18 +3449,18 @@
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A14" s="113" t="s">
+      <c r="A14" s="129" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="112"/>
+      <c r="B14" s="128"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="115" t="s">
+      <c r="F14" s="131" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="112"/>
-      <c r="H14" s="112"/>
+      <c r="G14" s="128"/>
+      <c r="H14" s="128"/>
       <c r="I14" s="5"/>
       <c r="J14" s="4"/>
     </row>
@@ -3621,8 +3615,8 @@
   </sheetPr>
   <dimension ref="A1:L659"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A278" workbookViewId="0">
-      <selection activeCell="J294" sqref="J294"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3654,15 +3648,15 @@
       <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" ht="12.75">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="127" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -3700,15 +3694,15 @@
       <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:12" ht="12.75">
-      <c r="A5" s="111" t="s">
+      <c r="A5" s="127" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="112"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
+      <c r="B5" s="128"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -3716,15 +3710,15 @@
       <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:12" ht="14.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="132" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
+      <c r="B6" s="128"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -3732,15 +3726,15 @@
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" ht="14.25">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="132" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="128"/>
+      <c r="D7" s="128"/>
+      <c r="E7" s="128"/>
+      <c r="F7" s="128"/>
+      <c r="G7" s="128"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -3762,16 +3756,16 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12" ht="14.25">
-      <c r="A9" s="116" t="s">
+      <c r="A9" s="132" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="112"/>
-      <c r="C9" s="112"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="112"/>
-      <c r="H9" s="112"/>
+      <c r="B9" s="128"/>
+      <c r="C9" s="128"/>
+      <c r="D9" s="128"/>
+      <c r="E9" s="128"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="128"/>
+      <c r="H9" s="128"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -4670,39 +4664,17 @@
       <c r="L36" s="4"/>
     </row>
     <row r="37" spans="1:12" ht="21.75">
-      <c r="A37" s="31" t="s">
-        <v>659</v>
-      </c>
-      <c r="B37" s="15">
-        <v>10</v>
-      </c>
-      <c r="C37" s="15">
-        <v>1</v>
-      </c>
-      <c r="D37" s="15">
-        <v>2</v>
-      </c>
-      <c r="E37" s="15">
-        <v>3</v>
-      </c>
-      <c r="F37" s="15">
-        <v>4</v>
-      </c>
-      <c r="G37" s="15">
-        <v>5</v>
-      </c>
-      <c r="H37" s="15">
-        <v>6</v>
-      </c>
-      <c r="I37" s="15">
-        <v>7</v>
-      </c>
-      <c r="J37" s="32">
-        <v>8</v>
-      </c>
-      <c r="K37" s="110" t="s">
-        <v>660</v>
-      </c>
+      <c r="A37" s="31"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="110"/>
       <c r="L37" s="4"/>
     </row>
     <row r="38" spans="1:12" ht="14.25">
@@ -6927,107 +6899,107 @@
       </c>
     </row>
     <row r="193" spans="1:11" ht="14.25">
-      <c r="A193" s="126" t="s">
+      <c r="A193" s="116" t="s">
         <v>174</v>
       </c>
-      <c r="B193" s="127">
+      <c r="B193" s="117">
         <v>78</v>
       </c>
-      <c r="C193" s="127">
+      <c r="C193" s="117">
         <v>2.1</v>
       </c>
-      <c r="D193" s="127">
+      <c r="D193" s="117">
         <v>7.3</v>
       </c>
-      <c r="E193" s="127">
+      <c r="E193" s="117">
         <v>7</v>
       </c>
-      <c r="F193" s="127">
+      <c r="F193" s="117">
         <v>6.2</v>
       </c>
-      <c r="G193" s="127">
+      <c r="G193" s="117">
         <v>0.2</v>
       </c>
-      <c r="H193" s="127">
+      <c r="H193" s="117">
         <v>13.3</v>
       </c>
-      <c r="I193" s="127">
+      <c r="I193" s="117">
         <v>13.5</v>
       </c>
-      <c r="J193" s="127">
+      <c r="J193" s="117">
         <v>1.9</v>
       </c>
-      <c r="K193" s="128" t="s">
+      <c r="K193" s="118" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="194" spans="1:11" ht="14.25">
-      <c r="A194" s="132" t="s">
-        <v>661</v>
-      </c>
-      <c r="B194" s="133">
+      <c r="A194" s="122" t="s">
+        <v>659</v>
+      </c>
+      <c r="B194" s="123">
         <v>78</v>
       </c>
-      <c r="C194" s="133">
+      <c r="C194" s="123">
         <v>1.3</v>
       </c>
-      <c r="D194" s="133">
+      <c r="D194" s="123">
         <v>5.6</v>
       </c>
-      <c r="E194" s="133">
+      <c r="E194" s="123">
         <v>4.3</v>
       </c>
-      <c r="F194" s="133">
+      <c r="F194" s="123">
         <v>11</v>
       </c>
-      <c r="G194" s="133">
+      <c r="G194" s="123">
         <v>0.71</v>
       </c>
-      <c r="H194" s="134">
+      <c r="H194" s="124">
         <v>13.138999999999999</v>
       </c>
-      <c r="I194" s="133">
+      <c r="I194" s="123">
         <v>6.6</v>
       </c>
-      <c r="J194" s="135">
+      <c r="J194" s="125">
         <v>1.3</v>
       </c>
-      <c r="K194" s="136" t="s">
+      <c r="K194" s="126" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="195" spans="1:11" ht="14.25">
-      <c r="A195" s="129" t="s">
+      <c r="A195" s="119" t="s">
         <v>175</v>
       </c>
-      <c r="B195" s="130">
+      <c r="B195" s="120">
         <v>103</v>
       </c>
-      <c r="C195" s="130">
+      <c r="C195" s="120">
         <v>3.2</v>
       </c>
-      <c r="D195" s="130">
+      <c r="D195" s="120">
         <v>15</v>
       </c>
-      <c r="E195" s="130">
+      <c r="E195" s="120">
         <v>13</v>
       </c>
-      <c r="F195" s="130">
+      <c r="F195" s="120">
         <v>3.6</v>
       </c>
-      <c r="G195" s="130">
+      <c r="G195" s="120">
         <v>0.12</v>
       </c>
-      <c r="H195" s="130">
+      <c r="H195" s="120">
         <v>13</v>
       </c>
-      <c r="I195" s="130">
+      <c r="I195" s="120">
         <v>18.600000000000001</v>
       </c>
-      <c r="J195" s="130">
+      <c r="J195" s="120">
         <v>2.9</v>
       </c>
-      <c r="K195" s="131" t="s">
+      <c r="K195" s="121" t="s">
         <v>176</v>
       </c>
     </row>
@@ -10277,20 +10249,20 @@
       </c>
     </row>
     <row r="291" spans="1:11" ht="15.75" customHeight="1">
-      <c r="E291" s="122"/>
+      <c r="E291" s="112"/>
     </row>
     <row r="292" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A292" s="121"/>
-      <c r="B292" s="122"/>
-      <c r="C292" s="122"/>
-      <c r="D292" s="122"/>
-      <c r="E292" s="122"/>
-      <c r="F292" s="122"/>
-      <c r="G292" s="122"/>
-      <c r="H292" s="124"/>
-      <c r="I292" s="122"/>
-      <c r="J292" s="123"/>
-      <c r="K292" s="125"/>
+      <c r="A292" s="111"/>
+      <c r="B292" s="112"/>
+      <c r="C292" s="112"/>
+      <c r="D292" s="112"/>
+      <c r="E292" s="112"/>
+      <c r="F292" s="112"/>
+      <c r="G292" s="112"/>
+      <c r="H292" s="114"/>
+      <c r="I292" s="112"/>
+      <c r="J292" s="113"/>
+      <c r="K292" s="115"/>
     </row>
     <row r="296" spans="1:11" ht="21.75">
       <c r="A296" s="61" t="s">
@@ -19972,26 +19944,26 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2D050267-7263-4CD4-97DE-20ADEF3AA056}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{BFC8CB06-61D4-4AB5-8D7C-32259655DEAE}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A63:K96" xr:uid="{97A59D0A-7D89-4CE1-B85C-DF9C144E3857}"/>
-    </customSheetView>
-    <customSheetView guid="{DDEA0034-8075-451D-A031-0121E8381F0F}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A13:K40" xr:uid="{C7BD5ABF-3BB9-44C5-B338-36AEA2040D07}"/>
+      <autoFilter ref="A63:K96" xr:uid="{65E557AC-0B5F-4106-9F06-DE3ADAEE3327}"/>
     </customSheetView>
     <customSheetView guid="{78FFC831-1D0F-4AD8-8D5F-BA4B980A515D}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A152:K164" xr:uid="{8E60E02A-DB9F-4F2A-A236-E4A670F2A469}">
+      <autoFilter ref="A152:K164" xr:uid="{2D47DD10-3FC5-413A-A7A4-225471EE04FD}">
         <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A152:K164">
           <sortCondition descending="1" ref="H152:H164"/>
           <sortCondition descending="1" ref="I152:I164"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{BFC8CB06-61D4-4AB5-8D7C-32259655DEAE}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{DDEA0034-8075-451D-A031-0121E8381F0F}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A63:K96" xr:uid="{8CD9B793-1BA8-481C-B8D9-21FE7676F071}"/>
+      <autoFilter ref="A13:K40" xr:uid="{3321610B-621C-46E1-A6B9-A4B76656BBB4}"/>
+    </customSheetView>
+    <customSheetView guid="{2D050267-7263-4CD4-97DE-20ADEF3AA056}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A63:K96" xr:uid="{E439C743-B806-4389-B3FE-4D6CF1E2F1C2}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="5">
@@ -20029,10 +20001,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="42">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="130" t="s">
         <v>633</v>
       </c>
-      <c r="B1" s="112"/>
+      <c r="B1" s="128"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -20061,11 +20033,11 @@
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="14.25">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="127" t="s">
         <v>634</v>
       </c>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
       <c r="D3" s="3"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -21210,12 +21182,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="42">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="134" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
       <c r="E1" s="92"/>
       <c r="F1" s="92"/>
       <c r="G1" s="92"/>
@@ -21226,16 +21198,16 @@
       <c r="L1" s="93"/>
     </row>
     <row r="2" spans="1:12" ht="12.75">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="133" t="s">
         <v>645</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
       <c r="I2" s="92"/>
       <c r="J2" s="92"/>
       <c r="K2" s="92"/>
@@ -21256,14 +21228,14 @@
       <c r="L3" s="93"/>
     </row>
     <row r="4" spans="1:12" ht="28.5">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="135" t="s">
         <v>646</v>
       </c>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="128"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
       <c r="G4" s="92"/>
       <c r="H4" s="92"/>
       <c r="I4" s="92"/>
@@ -21272,32 +21244,32 @@
       <c r="L4" s="93"/>
     </row>
     <row r="5" spans="1:12" ht="12.75">
-      <c r="A5" s="117" t="s">
+      <c r="A5" s="133" t="s">
         <v>647</v>
       </c>
-      <c r="B5" s="112"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="112"/>
+      <c r="B5" s="128"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="128"/>
       <c r="I5" s="92"/>
       <c r="J5" s="92"/>
       <c r="K5" s="92"/>
       <c r="L5" s="93"/>
     </row>
     <row r="6" spans="1:12" ht="14.25">
-      <c r="A6" s="120" t="s">
+      <c r="A6" s="136" t="s">
         <v>648</v>
       </c>
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
+      <c r="B6" s="128"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
       <c r="I6" s="92"/>
       <c r="J6" s="92"/>
       <c r="K6" s="92"/>
@@ -21318,10 +21290,10 @@
       <c r="L7" s="93"/>
     </row>
     <row r="8" spans="1:12" ht="28.5">
-      <c r="A8" s="119" t="s">
+      <c r="A8" s="135" t="s">
         <v>649</v>
       </c>
-      <c r="B8" s="112"/>
+      <c r="B8" s="128"/>
       <c r="C8" s="92"/>
       <c r="D8" s="92"/>
       <c r="E8" s="92"/>
@@ -21334,48 +21306,48 @@
       <c r="L8" s="93"/>
     </row>
     <row r="9" spans="1:12" ht="12.75">
-      <c r="A9" s="117" t="s">
+      <c r="A9" s="133" t="s">
         <v>650</v>
       </c>
-      <c r="B9" s="112"/>
-      <c r="C9" s="112"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="112"/>
-      <c r="H9" s="112"/>
+      <c r="B9" s="128"/>
+      <c r="C9" s="128"/>
+      <c r="D9" s="128"/>
+      <c r="E9" s="128"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="128"/>
+      <c r="H9" s="128"/>
       <c r="I9" s="92"/>
       <c r="J9" s="92"/>
       <c r="K9" s="92"/>
       <c r="L9" s="93"/>
     </row>
     <row r="10" spans="1:12" ht="12.75">
-      <c r="A10" s="117" t="s">
+      <c r="A10" s="133" t="s">
         <v>651</v>
       </c>
-      <c r="B10" s="112"/>
-      <c r="C10" s="112"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="112"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="112"/>
-      <c r="H10" s="112"/>
+      <c r="B10" s="128"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="128"/>
+      <c r="E10" s="128"/>
+      <c r="F10" s="128"/>
+      <c r="G10" s="128"/>
+      <c r="H10" s="128"/>
       <c r="I10" s="92"/>
       <c r="J10" s="92"/>
       <c r="K10" s="92"/>
       <c r="L10" s="93"/>
     </row>
     <row r="11" spans="1:12" ht="12.75">
-      <c r="A11" s="117" t="s">
+      <c r="A11" s="133" t="s">
         <v>652</v>
       </c>
-      <c r="B11" s="112"/>
-      <c r="C11" s="112"/>
-      <c r="D11" s="112"/>
-      <c r="E11" s="112"/>
-      <c r="F11" s="112"/>
-      <c r="G11" s="112"/>
-      <c r="H11" s="112"/>
+      <c r="B11" s="128"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="128"/>
+      <c r="F11" s="128"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="128"/>
       <c r="I11" s="92"/>
       <c r="J11" s="92"/>
       <c r="K11" s="92"/>
@@ -21396,10 +21368,10 @@
       <c r="L12" s="96"/>
     </row>
     <row r="13" spans="1:12" ht="28.5">
-      <c r="A13" s="119" t="s">
+      <c r="A13" s="135" t="s">
         <v>653</v>
       </c>
-      <c r="B13" s="112"/>
+      <c r="B13" s="128"/>
       <c r="C13" s="92"/>
       <c r="D13" s="92"/>
       <c r="E13" s="92"/>
@@ -21412,16 +21384,16 @@
       <c r="L13" s="98"/>
     </row>
     <row r="14" spans="1:12" ht="12.75">
-      <c r="A14" s="117" t="s">
+      <c r="A14" s="133" t="s">
         <v>654</v>
       </c>
-      <c r="B14" s="112"/>
-      <c r="C14" s="112"/>
-      <c r="D14" s="112"/>
-      <c r="E14" s="112"/>
-      <c r="F14" s="112"/>
-      <c r="G14" s="112"/>
-      <c r="H14" s="112"/>
+      <c r="B14" s="128"/>
+      <c r="C14" s="128"/>
+      <c r="D14" s="128"/>
+      <c r="E14" s="128"/>
+      <c r="F14" s="128"/>
+      <c r="G14" s="128"/>
+      <c r="H14" s="128"/>
       <c r="I14" s="92"/>
       <c r="J14" s="92"/>
       <c r="K14" s="92"/>
@@ -21442,11 +21414,11 @@
       <c r="L15" s="93"/>
     </row>
     <row r="16" spans="1:12" ht="28.5">
-      <c r="A16" s="119" t="s">
+      <c r="A16" s="135" t="s">
         <v>655</v>
       </c>
-      <c r="B16" s="112"/>
-      <c r="C16" s="112"/>
+      <c r="B16" s="128"/>
+      <c r="C16" s="128"/>
       <c r="D16" s="92"/>
       <c r="E16" s="92"/>
       <c r="F16" s="92"/>
@@ -21458,16 +21430,16 @@
       <c r="L16" s="93"/>
     </row>
     <row r="17" spans="1:12" ht="12.75">
-      <c r="A17" s="117" t="s">
+      <c r="A17" s="133" t="s">
         <v>656</v>
       </c>
-      <c r="B17" s="112"/>
-      <c r="C17" s="112"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="112"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="112"/>
+      <c r="B17" s="128"/>
+      <c r="C17" s="128"/>
+      <c r="D17" s="128"/>
+      <c r="E17" s="128"/>
+      <c r="F17" s="128"/>
+      <c r="G17" s="128"/>
+      <c r="H17" s="128"/>
       <c r="I17" s="92"/>
       <c r="J17" s="92"/>
       <c r="K17" s="92"/>
@@ -21488,16 +21460,16 @@
       <c r="L18" s="93"/>
     </row>
     <row r="19" spans="1:12" ht="12.75">
-      <c r="A19" s="117" t="s">
+      <c r="A19" s="133" t="s">
         <v>657</v>
       </c>
-      <c r="B19" s="112"/>
-      <c r="C19" s="112"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="112"/>
-      <c r="F19" s="112"/>
-      <c r="G19" s="112"/>
-      <c r="H19" s="112"/>
+      <c r="B19" s="128"/>
+      <c r="C19" s="128"/>
+      <c r="D19" s="128"/>
+      <c r="E19" s="128"/>
+      <c r="F19" s="128"/>
+      <c r="G19" s="128"/>
+      <c r="H19" s="128"/>
       <c r="I19" s="92"/>
       <c r="J19" s="92"/>
       <c r="K19" s="92"/>

</xml_diff>